<commit_message>
Remove OP Caps in Player Points
</commit_message>
<xml_diff>
--- a/CFC Fantasy League 2025.xlsx
+++ b/CFC Fantasy League 2025.xlsx
@@ -37,12 +37,12 @@
     <t>Tormented Titans</t>
   </si>
   <si>
+    <t>Gujju Gang</t>
+  </si>
+  <si>
     <t>La Furia Roja</t>
   </si>
   <si>
-    <t>Gujju Gang</t>
-  </si>
-  <si>
     <t>Raging Raptors</t>
   </si>
   <si>
@@ -55,24 +55,27 @@
     <t>Krunal Pandya</t>
   </si>
   <si>
+    <t>Sunil Narine</t>
+  </si>
+  <si>
     <t>Ajinkya Rahane</t>
   </si>
   <si>
+    <t>Philip Salt</t>
+  </si>
+  <si>
+    <t>Josh Hazlewood</t>
+  </si>
+  <si>
     <t>Virat Kohli</t>
   </si>
   <si>
-    <t>Sunil Narine</t>
-  </si>
-  <si>
-    <t>Philip Salt</t>
-  </si>
-  <si>
-    <t>Josh Hazlewood</t>
-  </si>
-  <si>
     <t>Rajat Patidar</t>
   </si>
   <si>
+    <t>Liam Livingstone</t>
+  </si>
+  <si>
     <t>Yash Dayal</t>
   </si>
   <si>
@@ -88,34 +91,31 @@
     <t>Jitesh Sharma</t>
   </si>
   <si>
+    <t>Rinku Singh</t>
+  </si>
+  <si>
     <t>Suyash Sharma</t>
   </si>
   <si>
-    <t>Rinku Singh</t>
+    <t>Devdutt Padikkal</t>
+  </si>
+  <si>
+    <t>Harshit Rana</t>
+  </si>
+  <si>
+    <t>Vaibhav Arora</t>
+  </si>
+  <si>
+    <t>Venkatesh Iyer</t>
+  </si>
+  <si>
+    <t>Quinton de Kock</t>
+  </si>
+  <si>
+    <t>Andre Russell</t>
   </si>
   <si>
     <t>Spencer Johnson</t>
-  </si>
-  <si>
-    <t>Liam Livingstone</t>
-  </si>
-  <si>
-    <t>Devdutt Padikkal</t>
-  </si>
-  <si>
-    <t>Harshit Rana</t>
-  </si>
-  <si>
-    <t>Vaibhav Arora</t>
-  </si>
-  <si>
-    <t>Venkatesh Iyer</t>
-  </si>
-  <si>
-    <t>Quinton de Kock</t>
-  </si>
-  <si>
-    <t>Andre Russell</t>
   </si>
   <si>
     <t>Tim David</t>
@@ -1095,7 +1095,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1104,7 +1104,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>446</v>
+        <v>448</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1129,7 +1129,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1138,7 +1138,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1146,7 +1146,7 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1155,7 +1155,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>240</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1197,7 +1197,7 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1206,7 +1206,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>69</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1241,13 +1241,13 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>667</v>
+        <v>167</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>167</v>
@@ -1258,16 +1258,16 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>635</v>
+        <v>148</v>
       </c>
       <c r="C3">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>135</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1275,16 +1275,16 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <v>631</v>
+        <v>135</v>
       </c>
       <c r="C4">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1292,7 +1292,7 @@
         <v>14</v>
       </c>
       <c r="B5">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1301,7 +1301,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>148</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1309,7 +1309,7 @@
         <v>15</v>
       </c>
       <c r="B6">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1318,7 +1318,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1326,7 +1326,7 @@
         <v>16</v>
       </c>
       <c r="B7">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1335,7 +1335,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1360,7 +1360,7 @@
         <v>18</v>
       </c>
       <c r="B9">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1369,7 +1369,7 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>59</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1377,7 +1377,7 @@
         <v>19</v>
       </c>
       <c r="B10">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1386,7 +1386,7 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1394,7 +1394,7 @@
         <v>20</v>
       </c>
       <c r="B11">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1403,7 +1403,7 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1411,7 +1411,7 @@
         <v>21</v>
       </c>
       <c r="B12">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1420,7 +1420,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1428,7 +1428,7 @@
         <v>22</v>
       </c>
       <c r="B13">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1437,7 +1437,7 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1445,7 +1445,7 @@
         <v>23</v>
       </c>
       <c r="B14">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1454,7 +1454,7 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1479,7 +1479,7 @@
         <v>25</v>
       </c>
       <c r="B16">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1488,7 +1488,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1496,7 +1496,7 @@
         <v>26</v>
       </c>
       <c r="B17">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1505,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1513,7 +1513,7 @@
         <v>27</v>
       </c>
       <c r="B18">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1522,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1530,7 +1530,7 @@
         <v>28</v>
       </c>
       <c r="B19">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1539,7 +1539,7 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1547,7 +1547,7 @@
         <v>29</v>
       </c>
       <c r="B20">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1556,7 +1556,7 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1564,7 +1564,7 @@
         <v>30</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1573,7 +1573,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1598,7 +1598,7 @@
         <v>32</v>
       </c>
       <c r="B23">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1607,7 +1607,7 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1772,7 +1772,7 @@
     </row>
     <row r="2" spans="1:38">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -1888,7 +1888,7 @@
     </row>
     <row r="3" spans="1:38">
       <c r="A3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -2004,7 +2004,7 @@
     </row>
     <row r="4" spans="1:38">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>135</v>
@@ -2236,7 +2236,7 @@
     </row>
     <row r="6" spans="1:38">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <v>57</v>
@@ -2352,7 +2352,7 @@
     </row>
     <row r="7" spans="1:38">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>148</v>
@@ -2468,7 +2468,7 @@
     </row>
     <row r="8" spans="1:38">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -2700,10 +2700,10 @@
     </row>
     <row r="10" spans="1:38">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B10">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -2745,7 +2745,7 @@
         <v>0</v>
       </c>
       <c r="P10">
-        <v>19</v>
+        <v>-6</v>
       </c>
       <c r="Q10">
         <v>0</v>
@@ -2766,10 +2766,10 @@
         <v>14</v>
       </c>
       <c r="W10">
-        <v>10.5</v>
+        <v>13.28</v>
       </c>
       <c r="X10">
-        <v>5</v>
+        <v>-20</v>
       </c>
       <c r="Y10">
         <v>0</v>
@@ -2816,7 +2816,7 @@
     </row>
     <row r="11" spans="1:38">
       <c r="A11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>20</v>
@@ -2932,7 +2932,7 @@
     </row>
     <row r="12" spans="1:38">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12">
         <v>44</v>
@@ -3048,10 +3048,10 @@
     </row>
     <row r="13" spans="1:38">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -3093,7 +3093,7 @@
         <v>0</v>
       </c>
       <c r="P13">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="Q13">
         <v>0</v>
@@ -3108,13 +3108,13 @@
         <v>25</v>
       </c>
       <c r="U13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V13">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="W13">
-        <v>15.37</v>
+        <v>14</v>
       </c>
       <c r="X13">
         <v>-20</v>
@@ -3164,7 +3164,7 @@
     </row>
     <row r="14" spans="1:38">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>131</v>
@@ -3280,7 +3280,7 @@
     </row>
     <row r="15" spans="1:38">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>135</v>
@@ -3512,10 +3512,10 @@
     </row>
     <row r="17" spans="1:38">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B17">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -3524,31 +3524,31 @@
         <v>73</v>
       </c>
       <c r="E17">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="F17">
+        <v>15</v>
+      </c>
+      <c r="G17">
+        <v>15</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
         <v>4</v>
       </c>
-      <c r="G17">
-        <v>4</v>
-      </c>
-      <c r="H17">
+      <c r="J17">
         <v>1</v>
       </c>
-      <c r="I17">
-        <v>2</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
       <c r="K17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L17">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="N17">
         <v>0</v>
@@ -3628,7 +3628,7 @@
     </row>
     <row r="18" spans="1:38">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>40</v>
@@ -3976,7 +3976,7 @@
     </row>
     <row r="21" spans="1:38">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>43</v>
@@ -4092,7 +4092,7 @@
     </row>
     <row r="22" spans="1:38">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B22">
         <v>39</v>
@@ -4208,7 +4208,7 @@
     </row>
     <row r="23" spans="1:38">
       <c r="A23" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B23">
         <v>132</v>
@@ -4324,7 +4324,7 @@
     </row>
     <row r="24" spans="1:38">
       <c r="A24" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B24">
         <v>59</v>
@@ -4440,7 +4440,7 @@
     </row>
     <row r="25" spans="1:38">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>27</v>
@@ -4575,13 +4575,13 @@
         <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>78</v>
@@ -4626,7 +4626,7 @@
         <v>91</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>92</v>
@@ -4692,7 +4692,7 @@
         <v>111</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="AR1" s="1" t="s">
         <v>112</v>
@@ -4743,7 +4743,7 @@
         <v>127</v>
       </c>
       <c r="BH1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="BI1" s="1" t="s">
         <v>128</v>
@@ -4752,7 +4752,7 @@
         <v>129</v>
       </c>
       <c r="BK1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="BL1" s="1" t="s">
         <v>130</v>
@@ -4764,7 +4764,7 @@
         <v>132</v>
       </c>
       <c r="BO1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="BP1" s="1" t="s">
         <v>133</v>
@@ -4809,7 +4809,7 @@
         <v>145</v>
       </c>
       <c r="CD1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="CE1" s="1" t="s">
         <v>146</v>
@@ -4836,7 +4836,7 @@
         <v>153</v>
       </c>
       <c r="CM1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="CN1" s="1" t="s">
         <v>154</v>
@@ -4851,7 +4851,7 @@
         <v>157</v>
       </c>
       <c r="CR1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="CS1" s="1" t="s">
         <v>158</v>
@@ -4863,7 +4863,7 @@
         <v>160</v>
       </c>
       <c r="CV1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="CW1" s="1" t="s">
         <v>161</v>
@@ -4878,7 +4878,7 @@
         <v>164</v>
       </c>
       <c r="DA1" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="DB1" s="1" t="s">
         <v>165</v>
@@ -4923,7 +4923,7 @@
         <v>178</v>
       </c>
       <c r="DP1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="DQ1" s="1" t="s">
         <v>179</v>
@@ -4974,7 +4974,7 @@
         <v>192</v>
       </c>
       <c r="EG1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="EH1" s="1" t="s">
         <v>193</v>
@@ -5004,7 +5004,7 @@
         <v>201</v>
       </c>
       <c r="EQ1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="ER1" s="1" t="s">
         <v>202</v>
@@ -5037,10 +5037,10 @@
         <v>210</v>
       </c>
       <c r="FB1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="FC1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="FD1" s="1" t="s">
         <v>211</v>
@@ -5055,7 +5055,7 @@
         <v>214</v>
       </c>
       <c r="FH1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="FI1" s="1" t="s">
         <v>215</v>
@@ -5085,7 +5085,7 @@
         <v>223</v>
       </c>
       <c r="FR1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="FS1" s="1" t="s">
         <v>224</v>
@@ -5111,7 +5111,7 @@
     </row>
     <row r="2" spans="1:181">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>240</v>
@@ -5659,7 +5659,7 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
         <v>231</v>
@@ -5782,7 +5782,7 @@
         <v>0</v>
       </c>
       <c r="AQ3">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="AR3">
         <v>0</v>
@@ -6746,10 +6746,10 @@
     </row>
     <row r="5" spans="1:181">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>247</v>
+        <v>222</v>
       </c>
       <c r="C5" t="s">
         <v>231</v>
@@ -7058,7 +7058,7 @@
         <v>0</v>
       </c>
       <c r="DA5">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="DB5">
         <v>0</v>
@@ -8384,7 +8384,7 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="C8" t="s">
         <v>231</v>
@@ -8900,7 +8900,7 @@
         <v>0</v>
       </c>
       <c r="FR8">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="FS8">
         <v>0</v>

</xml_diff>

<commit_message>
Man of the Match VC 45 Points
</commit_message>
<xml_diff>
--- a/CFC Fantasy League 2025.xlsx
+++ b/CFC Fantasy League 2025.xlsx
@@ -1095,7 +1095,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>448</v>
+        <v>453</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1104,7 +1104,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>448</v>
+        <v>453</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1163,7 +1163,7 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1172,7 +1172,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -7839,7 +7839,7 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="C7" t="s">
         <v>231</v>
@@ -8244,7 +8244,7 @@
         <v>0</v>
       </c>
       <c r="EG7">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="EH7">
         <v>0</v>
@@ -8384,7 +8384,7 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>448</v>
+        <v>453</v>
       </c>
       <c r="C8" t="s">
         <v>231</v>
@@ -8855,7 +8855,7 @@
         <v>296</v>
       </c>
       <c r="FC8">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="FD8">
         <v>0</v>

</xml_diff>